<commit_message>
updated cpp and ds
</commit_message>
<xml_diff>
--- a/interview_study/cpp/geeks_for_geeks_ds.xlsx
+++ b/interview_study/cpp/geeks_for_geeks_ds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\interview_preparation\cs_interview_prep\interview_study\cpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{16B21E65-960B-4747-9F1A-4E77ACD7DD76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF59A13C-B22F-48CB-8731-CD939D143056}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38670" windowHeight="11430" xr2:uid="{07024F4D-E5C7-4B8A-AB6A-143DE046C366}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="274">
   <si>
     <t>Topics</t>
   </si>
@@ -849,37 +849,6 @@
   </si>
   <si>
     <t>3. Expression Tree</t>
-  </si>
-  <si>
-    <r>
-      <t>Suffix Array and Suffix Tree</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <u/>
-        <sz val="11"/>
-        <color theme="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Suffix Array and Suffix Tree</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Var(--font-din)"/>
-      </rPr>
-      <t>:</t>
-    </r>
   </si>
   <si>
     <t>Suffix Array and Suffix Tree:</t>
@@ -1256,8 +1225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39FF427-EF33-4184-98B8-1EBCB416FB1F}">
   <dimension ref="C1:C302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
-      <selection activeCell="C302" sqref="C302"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1268,1442 +1237,1442 @@
     <col min="5" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="3:3" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="3:3" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C18" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C19" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C21" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C22" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C23" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C24" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C25" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C26" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C27" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C28" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C29" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="3:3" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C30" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C31" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C32" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C33" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C34" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C35" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C36" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="3:3" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C37" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C38" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C39" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C41" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C42" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C43" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C44" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C45" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C46" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C48" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C49" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C50" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C51" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C52" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C53" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C54" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C56" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C57" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C58" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C59" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C60" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C61" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C62" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C63" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C64" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="65" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C65" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="66" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C66" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="67" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C67" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="68" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C68" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C69" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="70" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C70" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="71" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C71" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="73" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C73" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C74" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="75" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C75" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="76" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C76" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="77" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C77" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="78" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C78" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="79" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C79" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="80" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="80" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C80" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="81" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C81" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="82" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C82" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="83" spans="3:3" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C83" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="84" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C84" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="86" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C86" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C87" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="88" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C88" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="89" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C89" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="90" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="90" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C90" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="91" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C91" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="92" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="92" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C92" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="93" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C93" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="94" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C94" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="95" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C95" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="96" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C96" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="97" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="97" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C97" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="98" spans="3:3" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="3:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C98" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="99" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C99" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="100" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="100" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C100" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="101" spans="3:3" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="3:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C101" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="102" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="102" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C102" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="103" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="103" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C103" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="104" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="104" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C104" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="105" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="105" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C105" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="106" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="106" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C106" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="107" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="107" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C107" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="108" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C108" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="110" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C110" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="111" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C111" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="112" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C112" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="113" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="113" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C113" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="114" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="114" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C114" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="115" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="115" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C115" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="116" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="116" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C116" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="117" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="117" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C117" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="118" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="118" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C118" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="119" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="119" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C119" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="120" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="120" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C120" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="121" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C121" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="122" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="122" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C122" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="123" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="123" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C123" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="124" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="124" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C124" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="125" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="125" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C125" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="126" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="126" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C126" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="128" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C128" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C129" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="130" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="130" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C130" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="131" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C131" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="132" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C132" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="133" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C133" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="134" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="134" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C134" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="135" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C135" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="136" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="136" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C136" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="138" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C138" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="139" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C139" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="140" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="140" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C140" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="141" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="141" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C141" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="142" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="142" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C142" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="143" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="143" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C143" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="144" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="144" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C144" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="145" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C145" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="146" spans="3:3" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="146" spans="3:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C146" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="147" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="147" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C147" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="148" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="148" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C148" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="150" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C150" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="151" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C151" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="152" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="152" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C152" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="153" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="153" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C153" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="154" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="154" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C154" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="155" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="155" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C155" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="156" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="156" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C156" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="157" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="157" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C157" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="158" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="158" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C158" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="159" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="159" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C159" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="160" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C160" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="161" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="161" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C161" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="162" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C162" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="163" spans="3:3" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="163" spans="3:3" ht="58" x14ac:dyDescent="0.35">
       <c r="C163" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="164" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="164" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C164" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="165" spans="3:3" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="165" spans="3:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C165" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="167" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C167" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="168" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C168" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="169" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="169" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C169" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="170" spans="3:3" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="170" spans="3:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C170" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="171" spans="3:3" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="171" spans="3:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C171" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="172" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C172" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="173" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="173" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C173" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="174" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="174" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C174" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="175" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C175" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="176" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="176" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C176" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="177" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="177" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C177" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="178" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="178" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C178" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="179" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="179" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C179" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="180" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C180" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="181" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C181" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="182" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C182" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="183" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C183" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="184" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="184" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C184" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="185" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="185" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C185" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="186" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="186" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C186" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="187" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="187" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C187" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="188" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C188" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="189" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C189" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="190" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C190" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="191" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="191" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C191" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="192" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="192" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C192" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="193" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="193" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C193" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="194" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="194" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C194" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="195" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C195" s="3" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="196" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="196" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C196" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="197" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C197" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="198" spans="3:3" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="198" spans="3:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C198" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="199" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C199" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="200" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="200" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C200" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="201" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="201" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C201" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="202" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="202" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C202" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="203" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="203" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C203" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="204" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="204" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C204" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="205" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="205" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C205" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="206" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C206" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="207" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="207" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C207" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="208" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C208" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="209" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C209" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="210" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C210" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="211" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="211" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C211" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="212" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C212" s="3"/>
     </row>
-    <row r="213" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C213" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="214" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C214" s="3" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="215" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C215" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="216" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C216" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="217" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C217" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="218" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C218" s="3" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="219" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C219" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="220" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C220" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="221" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C221" s="3" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="222" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C222" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="223" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C223" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="224" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C224" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="225" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C225" s="3" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="226" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C226" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="227" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C227" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="228" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C228" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="229" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="229" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C229" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="230" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C230" s="3"/>
     </row>
-    <row r="231" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="231" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C231" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="232" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C232" s="3"/>
     </row>
-    <row r="233" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C233" s="3" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="234" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C234" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="235" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C235" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="236" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C236" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="237" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C237" s="3" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="238" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="238" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C238" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="239" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C239" s="2" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="240" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C240" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="241" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C241" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="242" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="242" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C242" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="243" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="243" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C243" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="244" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="244" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C244" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="245" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="245" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C245" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="246" spans="3:3" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="246" spans="3:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C246" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="247" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C247" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="248" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="248" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C248" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="249" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="249" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C249" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="250" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="250" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C250" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="251" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C251" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="252" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="252" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C252" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="253" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C253" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="254" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="254" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C254" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="255" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C255" s="4" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="256" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="256" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C256" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="257" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="257" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C257" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="258" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="258" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C258" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="259" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="259" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C259" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="260" spans="3:3" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="260" spans="3:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C260" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="261" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="261" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C261" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="262" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="262" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C262" s="2" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="263" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="263" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C263" s="2" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="264" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="264" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C264" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="265" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="265" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C265" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="266" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="266" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C266" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="267" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C267" s="2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="268" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="268" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C268" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="269" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="269" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C269" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="270" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="270" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C270" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="271" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="271" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C271" s="2" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="272" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="272" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C272" s="2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="273" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="273" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C273" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="274" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="274" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C274" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="275" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="275" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C275" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="276" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="276" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C276" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="277" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="277" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C277" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="278" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="278" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C278" s="2" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="279" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="279" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C279" s="3"/>
     </row>
-    <row r="280" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="280" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C280" s="4" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="281" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="281" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C281" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="282" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="282" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C282" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="283" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="283" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C283" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="284" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="284" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C284" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="285" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="285" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C285" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="286" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="286" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C286" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="287" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="287" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C287" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="288" spans="3:3" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="288" spans="3:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C288" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="289" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="289" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C289" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="290" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="290" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C290" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="291" spans="3:3" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="291" spans="3:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C291" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="292" spans="3:3" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="292" spans="3:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C292" s="2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="293" spans="3:3" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="293" spans="3:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C293" s="2" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="294" spans="3:3" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="294" spans="3:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C294" s="2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="295" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="295" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C295" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="296" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="296" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C296" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="297" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="297" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C297" s="2" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="298" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="298" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C298" s="3"/>
     </row>
-    <row r="299" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="299" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C299" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="300" spans="3:3" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="300" spans="3:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C300" s="2" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="301" spans="3:3" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="301" spans="3:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C301" s="2" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="302" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="302" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C302" s="2" t="s">
         <v>272</v>
       </c>

</xml_diff>